<commit_message>
html and texcel know how to work with diseing and IsSummary row
</commit_message>
<xml_diff>
--- a/ReportTester/bin/Debug/net8.0/ArnSummaryComplexReport.xlsx
+++ b/ReportTester/bin/Debug/net8.0/ArnSummaryComplexReport.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>סיכום נתוני ארנונה</t>
   </si>
@@ -98,90 +98,183 @@
     <t>הסדר</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>444838.0000</t>
+  </si>
+  <si>
+    <t>-40.2000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>553</t>
+  </si>
+  <si>
+    <t>346</t>
+  </si>
+  <si>
+    <t>6817546.0000</t>
+  </si>
+  <si>
+    <t>-68862.3000</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>550</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>4653550.0000</t>
+  </si>
+  <si>
+    <t>0.0000</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>36940.4000</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>917</t>
+  </si>
+  <si>
+    <t>794</t>
+  </si>
+  <si>
+    <t>4128583.0000</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>קוד הנחה</t>
+  </si>
+  <si>
+    <t>תיאור ההנחה</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3983.2000</t>
-  </si>
-  <si>
-    <t>-40.2000</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>440854.8000</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>553</t>
-  </si>
-  <si>
-    <t>346</t>
-  </si>
-  <si>
-    <t>6817546.0000</t>
-  </si>
-  <si>
-    <t>-68862.3000</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>550</t>
-  </si>
-  <si>
-    <t>354</t>
-  </si>
-  <si>
-    <t>4653550.0000</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>36940.4000</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>917</t>
-  </si>
-  <si>
-    <t>794</t>
-  </si>
-  <si>
-    <t>4128583.0000</t>
-  </si>
-  <si>
-    <t>קוד הנחה</t>
-  </si>
-  <si>
-    <t>תיאור ההנחה</t>
-  </si>
-  <si>
     <t>-195.3000</t>
   </si>
   <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>100% הנחה-פטור(ועדה)</t>
+  </si>
+  <si>
+    <t>-515.2000</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>2/3-מ בטחון-קיבוצים</t>
+  </si>
+  <si>
+    <t>-55098.5000</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>25% א.ותיק מקבל ק.זיקנההנחה על 100 מ'ר</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>-194688.1000</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>25% הנחה פנסיונ (קבוצים)</t>
+  </si>
+  <si>
+    <t>-279846.0000</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>40% הנחה (הכנסה נמוכה)</t>
+  </si>
+  <si>
+    <t>-2721.6000</t>
+  </si>
+  <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>40% הנחה נכות רפואית מעל90%</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>-74383.3000</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>5% ל100 מ"ר הנחה למשרתי מילואים</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>-1724.3000</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>הנח2/3 נכות בשל רדיפות הנאצים-70מ"ר</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>-78766.9000</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>הנחה 10%הורה יחיד משותפת</t>
+  </si>
+  <si>
+    <t>-318.8000</t>
+  </si>
+  <si>
     <t>221</t>
   </si>
   <si>
@@ -194,34 +287,25 @@
     <t>-109031.3000</t>
   </si>
   <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>הנחה 10%הורה יחיד משותפת</t>
-  </si>
-  <si>
-    <t>-318.8000</t>
-  </si>
-  <si>
-    <t>225</t>
-  </si>
-  <si>
-    <t>25% א.ותיק מקבל ק.זיקנההנחה על 100 מ'ר</t>
-  </si>
-  <si>
-    <t>216</t>
-  </si>
-  <si>
-    <t>-194688.1000</t>
-  </si>
-  <si>
-    <t>226</t>
-  </si>
-  <si>
-    <t>25% הנחה פנסיונ (קבוצים)</t>
-  </si>
-  <si>
-    <t>-279846.0000</t>
+    <t>297</t>
+  </si>
+  <si>
+    <t>הנחה 66% נכס ריק</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>-55778.0000</t>
+  </si>
+  <si>
+    <t>293</t>
+  </si>
+  <si>
+    <t>הנחה לפי סיעף 5ג(ה)(6)</t>
+  </si>
+  <si>
+    <t>-1731.0200</t>
   </si>
   <si>
     <t>233</t>
@@ -233,25 +317,76 @@
     <t>-11142.9000</t>
   </si>
   <si>
-    <t>234</t>
-  </si>
-  <si>
-    <t>2/3-מ בטחון-קיבוצים</t>
-  </si>
-  <si>
-    <t>-55098.5000</t>
-  </si>
-  <si>
-    <t>237</t>
-  </si>
-  <si>
-    <t>הנח2/3 נכות בשל רדיפות הנאצים-70מ"ר</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>-78766.9000</t>
+    <t>280</t>
+  </si>
+  <si>
+    <t>הנחה80%(הכנ.נמוכה)</t>
+  </si>
+  <si>
+    <t>-4522.5000</t>
+  </si>
+  <si>
+    <t>282</t>
+  </si>
+  <si>
+    <t>הנחת נכות 80%</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>-407374.4000</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>הנחת סיעוד 70%</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>-503265.7000</t>
+  </si>
+  <si>
+    <t>2271</t>
+  </si>
+  <si>
+    <t>ילדים נכים-הנחה33%ל100מ"ר</t>
+  </si>
+  <si>
+    <t>-50381.9000</t>
+  </si>
+  <si>
+    <t>2281</t>
+  </si>
+  <si>
+    <t>ילדים נכים-הנחה33%-קבוצים</t>
+  </si>
+  <si>
+    <t>-30602.9000</t>
+  </si>
+  <si>
+    <t>303</t>
+  </si>
+  <si>
+    <t>נכה שהגיע לגיל זיקנה</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>-10368.1000</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>נכה שהגיע לגיל זיקנה-קיבוצים</t>
+  </si>
+  <si>
+    <t>-72828.0000</t>
   </si>
   <si>
     <t>238</t>
@@ -278,25 +413,34 @@
     <t>-30901.1000</t>
   </si>
   <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>40% הנחה (הכנסה נמוכה)</t>
-  </si>
-  <si>
-    <t>-2721.6000</t>
-  </si>
-  <si>
-    <t>241</t>
-  </si>
-  <si>
-    <t>40% הנחה נכות רפואית מעל90%</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>-74383.3000</t>
+    <t>300</t>
+  </si>
+  <si>
+    <t>נפגעי פעולות איבה 2/3 ל- 70 מ'</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>-4783.4000</t>
+  </si>
+  <si>
+    <t>291</t>
+  </si>
+  <si>
+    <t>עולה חדש הנחה90% קבוצים</t>
+  </si>
+  <si>
+    <t>-183.8000</t>
+  </si>
+  <si>
+    <t>296</t>
+  </si>
+  <si>
+    <t>פטור חיילים ל70מ'ר</t>
+  </si>
+  <si>
+    <t>-6841.3500</t>
   </si>
   <si>
     <t>267</t>
@@ -308,81 +452,6 @@
     <t>-2910.9000</t>
   </si>
   <si>
-    <t>270</t>
-  </si>
-  <si>
-    <t>הנחת סיעוד 70%</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>-503265.7000</t>
-  </si>
-  <si>
-    <t>280</t>
-  </si>
-  <si>
-    <t>הנחה80%(הכנ.נמוכה)</t>
-  </si>
-  <si>
-    <t>-4522.5000</t>
-  </si>
-  <si>
-    <t>282</t>
-  </si>
-  <si>
-    <t>הנחת נכות 80%</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>-407374.4000</t>
-  </si>
-  <si>
-    <t>291</t>
-  </si>
-  <si>
-    <t>עולה חדש הנחה90% קבוצים</t>
-  </si>
-  <si>
-    <t>-183.8000</t>
-  </si>
-  <si>
-    <t>293</t>
-  </si>
-  <si>
-    <t>הנחה לפי סיעף 5ג(ה)(6)</t>
-  </si>
-  <si>
-    <t>-1731.0200</t>
-  </si>
-  <si>
-    <t>296</t>
-  </si>
-  <si>
-    <t>פטור חיילים ל70מ'ר</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>-6841.3500</t>
-  </si>
-  <si>
-    <t>297</t>
-  </si>
-  <si>
-    <t>הנחה 66% נכס ריק</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>-55778.0000</t>
-  </si>
-  <si>
     <t>298</t>
   </si>
   <si>
@@ -392,73 +461,13 @@
     <t>-4629.8000</t>
   </si>
   <si>
-    <t>299</t>
-  </si>
-  <si>
-    <t>100% הנחה-פטור(ועדה)</t>
-  </si>
-  <si>
-    <t>-515.2000</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>נפגעי פעולות איבה 2/3 ל- 70 מ'</t>
-  </si>
-  <si>
-    <t>-4783.4000</t>
-  </si>
-  <si>
-    <t>303</t>
-  </si>
-  <si>
-    <t>נכה שהגיע לגיל זיקנה</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>-10368.1000</t>
-  </si>
-  <si>
-    <t>304</t>
-  </si>
-  <si>
-    <t>נכה שהגיע לגיל זיקנה-קיבוצים</t>
-  </si>
-  <si>
-    <t>-72828.0000</t>
-  </si>
-  <si>
-    <t>305</t>
-  </si>
-  <si>
-    <t>5% ל100 מ"ר הנחה למשרתי מילואים</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>-1724.3000</t>
-  </si>
-  <si>
-    <t>2271</t>
-  </si>
-  <si>
-    <t>ילדים נכים-הנחה33%ל100מ"ר</t>
-  </si>
-  <si>
-    <t>-50381.9000</t>
-  </si>
-  <si>
-    <t>2281</t>
-  </si>
-  <si>
-    <t>ילדים נכים-הנחה33%-קבוצים</t>
-  </si>
-  <si>
-    <t>-30602.9000</t>
+    <t>שורת סיכום</t>
+  </si>
+  <si>
+    <t>595</t>
+  </si>
+  <si>
+    <t>-2076969.8700</t>
   </si>
 </sst>
 </file>
@@ -466,7 +475,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -481,8 +490,14 @@
       <sz val="14"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0055AA"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,6 +507,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F8FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -514,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -524,6 +544,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" borderId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,104 +781,104 @@
         <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>
@@ -865,7 +886,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="1"/>
   </sheetViews>
@@ -889,10 +910,10 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
@@ -903,13 +924,13 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>54</v>
@@ -923,77 +944,77 @@
         <v>56</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>74</v>
@@ -1035,21 +1056,21 @@
         <v>84</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>89</v>
@@ -1077,7 +1098,7 @@
         <v>95</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>96</v>
@@ -1091,49 +1112,49 @@
         <v>98</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>110</v>
@@ -1147,7 +1168,7 @@
         <v>112</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>113</v>
@@ -1161,49 +1182,49 @@
         <v>115</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>127</v>
@@ -1217,49 +1238,49 @@
         <v>129</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>141</v>
@@ -1273,7 +1294,7 @@
         <v>143</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>144</v>
@@ -1287,16 +1308,30 @@
         <v>146</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>147</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>